<commit_message>
Regulador de 3.3V independiente para PCB_D
</commit_message>
<xml_diff>
--- a/Hardware/Satelite/PCB_D/BOM_D.xlsx
+++ b/Hardware/Satelite/PCB_D/BOM_D.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys32\home\tmax4\esp\Hardware\Satelite\PCB_D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{281C92DC-FF19-4719-AB1D-43157FBF1EC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175D1EBF-5BDF-4581-8C19-61AD217BBA5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB_D" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="99">
   <si>
     <t>Qty</t>
   </si>
@@ -94,9 +94,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>RS1A-E3/5AT</t>
   </si>
   <si>
@@ -287,16 +284,49 @@
   </si>
   <si>
     <t>R5, R6</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>1uH</t>
+  </si>
+  <si>
+    <t>LQM21PN1R0MC0D</t>
+  </si>
+  <si>
+    <t>D4, D8</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>C2012X7R1A106M125AC</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>ADP2108AUJ-3.3</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:TSOT-23-5</t>
+  </si>
+  <si>
+    <t>ADP2108AUJZ-3.3-R7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,6 +457,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -773,7 +811,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -781,6 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -840,14 +879,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E25" totalsRowShown="0">
-  <autoFilter ref="A1:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:E28" totalsRowShown="0">
+  <autoFilter ref="A1:E28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Qty"/>
-    <tableColumn id="2" name="Reference(s)"/>
-    <tableColumn id="3" name="Value"/>
-    <tableColumn id="4" name="Footprint"/>
-    <tableColumn id="5" name="Manufacturer Part Number"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reference(s)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Footprint"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Manufacturer Part Number"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1149,12 +1188,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1235,19 +1274,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1255,16 +1294,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,16 +1311,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1289,84 +1328,84 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1">
-        <v>61300311121</v>
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="E11" s="1">
+        <v>61300311121</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1374,16 +1413,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1391,33 +1430,33 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
         <v>46</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,64 +1464,64 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
+      <c r="A17" s="3">
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1490,50 +1529,50 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="2">
-        <v>220</v>
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
       </c>
       <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
         <v>58</v>
-      </c>
-      <c r="E20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" t="s">
-        <v>68</v>
+        <v>87</v>
+      </c>
+      <c r="C22" s="2">
+        <v>220</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1541,16 +1580,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,16 +1597,16 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1575,22 +1614,74 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
         <v>78</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D27" t="s">
         <v>79</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E27" t="s">
         <v>80</v>
       </c>
-      <c r="E25" t="s">
-        <v>81</v>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>